<commit_message>
"join" is better than "merge" lol
- YouTube and Soundcloud collection functions fixed: using a "merge" instead of a "join" ended up deleting songs from the dataset.

- Tidying of the repository.

+ minor changes
</commit_message>
<xml_diff>
--- a/Monthly_Reports/Monthly_Data/2021 Charts Month 2.xlsx
+++ b/Monthly_Reports/Monthly_Data/2021 Charts Month 2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
   <si>
     <t>Artist</t>
   </si>
@@ -36,6 +36,9 @@
     <t>YouTube_Views</t>
   </si>
   <si>
+    <t>Martin Garrix, Tove Lo</t>
+  </si>
+  <si>
     <t>Feint</t>
   </si>
   <si>
@@ -45,6 +48,9 @@
     <t>Bleu Clair, OOTORO</t>
   </si>
   <si>
+    <t>Pressure</t>
+  </si>
+  <si>
     <t>Do Better</t>
   </si>
   <si>
@@ -54,12 +60,12 @@
     <t>Beat Like This</t>
   </si>
   <si>
+    <t>STMPD RCRDS</t>
+  </si>
+  <si>
     <t>Monstercat</t>
   </si>
   <si>
-    <t>STMPD RCRDS</t>
-  </si>
-  <si>
     <t>1001T_Supports</t>
   </si>
   <si>
@@ -67,6 +73,12 @@
   </si>
   <si>
     <t>Soundcloud_Plays</t>
+  </si>
+  <si>
+    <t>Martin Garrix</t>
+  </si>
+  <si>
+    <t>Tove Lo</t>
   </si>
   <si>
     <t>Teddy Killerz</t>
@@ -436,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,13 +473,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>51223</v>
+        <v>1286202</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -475,13 +487,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>49221</v>
+        <v>63216</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -489,13 +501,27 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>57445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>30311</v>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>40680</v>
       </c>
     </row>
   </sheetData>
@@ -505,7 +531,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -522,27 +548,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E2">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -550,33 +576,50 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>2</v>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +629,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -603,7 +646,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -611,41 +654,55 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>25301</v>
+        <v>59108</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>20536</v>
+        <v>33805</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>32523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>18231</v>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>25372</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +712,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -671,42 +728,58 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>51223</v>
+        <v>1286202</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>49221</v>
+        <v>1286202</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>49221</v>
+        <v>63216</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>30311</v>
+        <v>57445</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>30311</v>
+        <v>57445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>40680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>40680</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +789,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -727,65 +800,87 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C2">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>2</v>
+      <c r="C8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -795,7 +890,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -806,47 +901,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>25301</v>
+        <v>59108</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>20536</v>
+        <v>59108</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>20536</v>
+        <v>33805</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>18231</v>
+        <v>32523</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>18231</v>
+        <v>32523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>25372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>25372</v>
       </c>
     </row>
   </sheetData>
@@ -872,18 +983,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>100444</v>
+        <v>1326882</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>30311</v>
+        <v>120661</v>
       </c>
     </row>
   </sheetData>
@@ -904,32 +1015,32 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C2">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -950,23 +1061,23 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>43532</v>
+        <v>91631</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>20536</v>
+        <v>59177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>